<commit_message>
input validation in login page on client side
</commit_message>
<xml_diff>
--- a/MusicCamp/ExcelData/data.xlsx
+++ b/MusicCamp/ExcelData/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S525021\Downloads\Masters\Sem4\GDP\Student_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s525250\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added changes to edit master schedule
</commit_message>
<xml_diff>
--- a/MusicCamp/ExcelData/data.xlsx
+++ b/MusicCamp/ExcelData/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s525250\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S525021\Downloads\Masters\Sem4\GDP\Student_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented Logic for User registration, adding valid users to userLogin
</commit_message>
<xml_diff>
--- a/MusicCamp/ExcelData/data.xlsx
+++ b/MusicCamp/ExcelData/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s525250\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S525021\Downloads\Masters\Sem4\GDP\Student_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Student Schedule Done in User Module
</commit_message>
<xml_diff>
--- a/MusicCamp/ExcelData/data.xlsx
+++ b/MusicCamp/ExcelData/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S525021\Downloads\Masters\Sem4\GDP\Student_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s525250\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>